<commit_message>
Category editing, spreadsheet creation in app, elo rating bug fix.
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u1376967/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u1376967/Desktop/Programming crap/Rust crap/media_rating/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C2685C-D4CD-D947-BF61-1FA56191B284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCC8DC0-F566-B241-9796-04F547A5C889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="26400" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranked" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Movies</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>The Legend of Zelda: Skyward Sword</t>
-  </si>
-  <si>
-    <t>The Legend of Zelda: Twilight Princess</t>
   </si>
   <si>
     <t>The Legend of Zelda: Link's Awakening</t>
@@ -466,13 +463,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+    <col min="10" max="10" width="25.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -482,10 +485,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -499,19 +502,19 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -525,19 +528,19 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -551,19 +554,19 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -577,19 +580,19 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -603,19 +606,19 @@
         <v>13</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -629,19 +632,19 @@
         <v>14</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -655,7 +658,7 @@
         <v>15</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -664,18 +667,10 @@
         <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8">
         <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>